<commit_message>
Refine code: no need delete output.xlsx manunally
1. Always merge first sheet
2. No need delete output.xlsx manunally
</commit_message>
<xml_diff>
--- a/test_a.xlsx
+++ b/test_a.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="285" yWindow="90" windowWidth="9540" windowHeight="4515"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="test_a_sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -457,7 +457,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C4"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>